<commit_message>
Updated seeds for transactions
</commit_message>
<xml_diff>
--- a/usmart_energy_site/seed_files/user_seed.xlsx
+++ b/usmart_energy_site/seed_files/user_seed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pstewy/Documents/SeniorCollege/SeniorCapstoneProject/code/usmart-energy/usmart_energy_site/seed_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9672E5F5-D6B8-0143-9E87-907F5E0B9F5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBECCE4-3BD9-FA49-B236-0404D82079FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="15140" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_seed" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Stewart</t>
   </si>
@@ -28,20 +28,23 @@
     <t>pman@advanceddv.com</t>
   </si>
   <si>
-    <t>panel</t>
-  </si>
-  <si>
     <t>2213 E 2100 S</t>
   </si>
   <si>
     <t>Parker</t>
+  </si>
+  <si>
+    <t>Salt Lake City</t>
+  </si>
+  <si>
+    <t>Utah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,6 +175,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -474,7 +485,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -517,11 +528,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -555,6 +568,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -875,15 +889,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="A2:F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -895,8 +911,26 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>84102</v>
+      </c>
+      <c r="H1">
+        <v>40.72589</v>
+      </c>
+      <c r="I1">
+        <v>-111.82782</v>
+      </c>
+      <c r="J1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>